<commit_message>
Add: multiple more sheets
</commit_message>
<xml_diff>
--- a/finalSheet.xlsx
+++ b/finalSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zamin\Git Projects\DataMiningFinalProj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED7D4A46-8A10-4565-BD62-62EB9DC285C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DFA02B-C5F4-4212-9A63-1F529D0CF77C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_country_attributes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">Table6!$A$1:$FK$16386</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30690,7 +30689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N168"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -38146,7 +38145,7 @@
         <v>3475842</v>
       </c>
       <c r="M162" s="1">
-        <f t="shared" ref="M162:M193" si="8">K162/L162</f>
+        <f t="shared" ref="M162:M168" si="8">K162/L162</f>
         <v>0.16622936255445442</v>
       </c>
       <c r="N162" s="2">
@@ -38444,7 +38443,7 @@
   <dimension ref="B1:O168"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43799,7 +43798,7 @@
         <v>51900</v>
       </c>
       <c r="K162" s="8">
-        <f t="shared" ref="K162:K193" si="5">I162/J162</f>
+        <f t="shared" ref="K162:K168" si="5">I162/J162</f>
         <v>1.1868978805394991E-4</v>
       </c>
     </row>
@@ -44010,7 +44009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>

</xml_diff>